<commit_message>
Alle mine noter fra Excel-arket er lavet. + tilkoblet RankedIn-ID
</commit_message>
<xml_diff>
--- a/Documentation/Notifications + small notes.xlsx
+++ b/Documentation/Notifications + small notes.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="202300"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://viaucdk-my.sharepoint.com/personal/331187_viauc_dk/Documents/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\IdeaProjects\smashpadelcenter\Documentation\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{BBD398F0-DBA1-4358-BF72-90D4328B5276}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D260FEF9-BAFA-4CE9-971F-18BAA89AF48B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-110" yWindow="-110" windowWidth="25820" windowHeight="15500" xr2:uid="{BB2EBD8B-0173-4FDD-B1E8-BD06B888A15E}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="38640" windowHeight="21240" xr2:uid="{BB2EBD8B-0173-4FDD-B1E8-BD06B888A15E}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="34" uniqueCount="32">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="40" uniqueCount="33">
   <si>
     <t xml:space="preserve">Notiification: </t>
   </si>
@@ -132,6 +132,9 @@
   </si>
   <si>
     <t>Kig på margin mellem baneoversigt og info på små telefoner</t>
+  </si>
+  <si>
+    <t>Done</t>
   </si>
 </sst>
 </file>
@@ -187,7 +190,7 @@
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office-tema">
   <a:themeElements>
     <a:clrScheme name="Office">
       <a:dk1>
@@ -503,22 +506,23 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{7389B0EF-A515-404E-B379-30B289523D1B}">
-  <dimension ref="A1:F14"/>
+  <dimension ref="A1:G14"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F14" sqref="F14"/>
+      <selection activeCell="F17" sqref="F17"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="69" customWidth="1"/>
-    <col min="2" max="2" width="23.7265625" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="12.7265625" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="19.81640625" customWidth="1"/>
-    <col min="6" max="6" width="48.81640625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="30" customWidth="1"/>
+    <col min="3" max="3" width="12.7109375" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="19.85546875" customWidth="1"/>
+    <col min="6" max="6" width="65" customWidth="1"/>
+    <col min="7" max="7" width="12.28515625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -531,8 +535,11 @@
       <c r="F1" t="s">
         <v>2</v>
       </c>
-    </row>
-    <row r="2" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="G1" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="2" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>8</v>
       </c>
@@ -543,7 +550,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="3" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="3" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>12</v>
       </c>
@@ -554,7 +561,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="4" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="4" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>15</v>
       </c>
@@ -565,7 +572,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="5" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="5" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
         <v>16</v>
       </c>
@@ -573,7 +580,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="6" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="6" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
         <v>18</v>
       </c>
@@ -583,8 +590,11 @@
       <c r="F6" t="s">
         <v>3</v>
       </c>
-    </row>
-    <row r="7" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="G6" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="7" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
         <v>20</v>
       </c>
@@ -594,8 +604,11 @@
       <c r="F7" t="s">
         <v>4</v>
       </c>
-    </row>
-    <row r="8" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="G7" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="8" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
         <v>22</v>
       </c>
@@ -605,8 +618,11 @@
       <c r="F8" t="s">
         <v>5</v>
       </c>
-    </row>
-    <row r="9" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="G8" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="9" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
         <v>21</v>
       </c>
@@ -616,13 +632,19 @@
       <c r="F9" t="s">
         <v>31</v>
       </c>
-    </row>
-    <row r="11" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="G9" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="11" spans="1:7" x14ac:dyDescent="0.25">
       <c r="F11" t="s">
         <v>24</v>
       </c>
-    </row>
-    <row r="12" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="G11" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="12" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
         <v>25</v>
       </c>
@@ -630,7 +652,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="13" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="13" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
         <v>29</v>
       </c>
@@ -638,7 +660,7 @@
         <v>30</v>
       </c>
     </row>
-    <row r="14" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="14" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
         <v>28</v>
       </c>
@@ -891,20 +913,20 @@
 </file>
 
 <file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
+<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+  <documentManagement>
+    <_activity xmlns="9750baf7-fcf3-4f7a-b82f-a9f904572e35" xsi:nil="true"/>
+  </documentManagement>
+</p:properties>
+</file>
+
+<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
 <?mso-contentType ?>
 <FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
   <Display>DocumentLibraryForm</Display>
   <Edit>DocumentLibraryForm</Edit>
   <New>DocumentLibraryForm</New>
 </FormTemplates>
-</file>
-
-<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
-<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
-  <documentManagement>
-    <_activity xmlns="9750baf7-fcf3-4f7a-b82f-a9f904572e35" xsi:nil="true"/>
-  </documentManagement>
-</p:properties>
 </file>
 
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -927,14 +949,6 @@
 </file>
 
 <file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{0F066BFA-AB8F-4D7E-B5E8-3517F6E2DFFE}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
-</file>
-
-<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{39EA4783-BC45-485E-965E-A5D8BAD4BE41}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="8b1a0762-17ff-4761-90b1-4f66cbf6cc52"/>
@@ -949,4 +963,12 @@
     <ds:schemaRef ds:uri="http://purl.org/dc/dcmitype/"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
+</file>
+
+<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{0F066BFA-AB8F-4D7E-B5E8-3517F6E2DFFE}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
 </file>
</xml_diff>